<commit_message>
final commit of upload excel file
</commit_message>
<xml_diff>
--- a/assets/uploads/contactDetail (16)11.xlsx
+++ b/assets/uploads/contactDetail (16)11.xlsx
@@ -55,7 +55,7 @@
     <t>Miss</t>
   </si>
   <si>
-    <t/>
+    <t>rohan</t>
   </si>
   <si>
     <t>S</t>
@@ -76,13 +76,13 @@
     <t>M G Street</t>
   </si>
   <si>
-    <t>lini@gmail.com</t>
-  </si>
-  <si>
-    <t>Reading ,Drawing ,</t>
-  </si>
-  <si>
-    <t>Maya</t>
+    <t>tintu@gmail.com</t>
+  </si>
+  <si>
+    <t>Reading ,Drawing</t>
+  </si>
+  <si>
+    <t>mini</t>
   </si>
   <si>
     <t>2024-06-20</t>
@@ -94,13 +94,13 @@
     <t>dfgdb</t>
   </si>
   <si>
-    <t>dfbdf</t>
+    <t>abcd</t>
   </si>
   <si>
     <t>maya@gmail.com</t>
   </si>
   <si>
-    <t>Reading ,Writing ,</t>
+    <t>Reading ,Writing</t>
   </si>
 </sst>
 </file>
@@ -118,7 +118,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -150,15 +150,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -478,21 +472,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="5.147857142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="7.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="45.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="5.147857142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="10.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="7.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="45.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="3" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="8.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="3" width="17.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="4" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="3" width="17.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -530,11 +524,11 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -555,20 +549,20 @@
       <c r="H2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="2">
         <v>695004</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="2">
         <v>9323415243</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -593,13 +587,13 @@
       <c r="H3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="2">
         <v>695004</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="2">
         <v>919523415000</v>
       </c>
       <c r="L3" s="1" t="s">

</xml_diff>